<commit_message>
minor tweaks/readability fix; finish report
</commit_message>
<xml_diff>
--- a/neuralnets/twentyq/files/spreadsheets/initialconcepts.xlsx
+++ b/neuralnets/twentyq/files/spreadsheets/initialconcepts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="26">
   <si>
     <t>Output</t>
   </si>
@@ -45,6 +45,54 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Dog</t>
+  </si>
+  <si>
+    <t>Human</t>
+  </si>
+  <si>
+    <t>Pig</t>
+  </si>
+  <si>
+    <t>Bat</t>
+  </si>
+  <si>
+    <t>Tiger</t>
+  </si>
+  <si>
+    <t>Rat</t>
+  </si>
+  <si>
+    <t>Deer</t>
+  </si>
+  <si>
+    <t>Giraffe</t>
+  </si>
+  <si>
+    <t>Monkey</t>
+  </si>
+  <si>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>Turtle</t>
+  </si>
+  <si>
+    <t>Lizard</t>
+  </si>
+  <si>
+    <t>Shark</t>
+  </si>
+  <si>
+    <t>Penguin</t>
+  </si>
+  <si>
+    <t>Bird</t>
+  </si>
+  <si>
+    <t>Snake</t>
   </si>
 </sst>
 </file>
@@ -222,20 +270,20 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.0714285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1224489795918"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.484693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.4948979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="16.219387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.0612244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.8775510204082"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.6275510204082"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -679,6 +727,134 @@
       </c>
       <c r="H17" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>